<commit_message>
adding sims to short list
</commit_message>
<xml_diff>
--- a/LOCA2_inventory_full.xlsx
+++ b/LOCA2_inventory_full.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/LOCA2_Prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C6CF44-C883-5D48-94BD-53FE08DF0571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881BFC36-223C-CE48-97E1-CA693570E1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1041,7 +1041,7 @@
   <dimension ref="A1:G2701"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2604" sqref="K2604"/>
+      <selection activeCell="G2698" sqref="A1:G2698"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -60757,7 +60757,7 @@
         <v>6.49846135635197</v>
       </c>
     </row>
-    <row r="2597" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2597" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2597" t="s">
         <v>27</v>
       </c>
@@ -60803,7 +60803,7 @@
         <v>6.6588287258345904</v>
       </c>
     </row>
-    <row r="2599" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2599" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2599" t="s">
         <v>30</v>
       </c>
@@ -60826,7 +60826,7 @@
         <v>6.68131723539602</v>
       </c>
     </row>
-    <row r="2600" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2600" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2600" t="s">
         <v>29</v>
       </c>
@@ -60895,7 +60895,7 @@
         <v>8.1657822650374392</v>
       </c>
     </row>
-    <row r="2603" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2603" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2603" t="s">
         <v>49</v>
       </c>
@@ -60918,7 +60918,7 @@
         <v>9.3994680700558799</v>
       </c>
     </row>
-    <row r="2604" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2604" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2604" t="s">
         <v>43</v>
       </c>
@@ -60941,7 +60941,7 @@
         <v>9.5958324287161201</v>
       </c>
     </row>
-    <row r="2605" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2605" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2605" t="s">
         <v>41</v>
       </c>
@@ -60964,7 +60964,7 @@
         <v>9.7308786859152594</v>
       </c>
     </row>
-    <row r="2606" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2606" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2606" t="s">
         <v>43</v>
       </c>
@@ -60987,7 +60987,7 @@
         <v>9.8483501156285005</v>
       </c>
     </row>
-    <row r="2607" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2607" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2607" t="s">
         <v>51</v>
       </c>
@@ -61079,7 +61079,7 @@
         <v>10.193134944657601</v>
       </c>
     </row>
-    <row r="2611" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2611" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2611" t="s">
         <v>37</v>
       </c>
@@ -61125,7 +61125,7 @@
         <v>9.9206854601887198</v>
       </c>
     </row>
-    <row r="2613" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2613" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2613" t="s">
         <v>50</v>
       </c>
@@ -61148,7 +61148,7 @@
         <v>9.9020199959402202</v>
       </c>
     </row>
-    <row r="2614" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2614" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2614" t="s">
         <v>34</v>
       </c>
@@ -61171,7 +61171,7 @@
         <v>9.9307602931497598</v>
       </c>
     </row>
-    <row r="2615" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2615" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2615" t="s">
         <v>50</v>
       </c>
@@ -61217,7 +61217,7 @@
         <v>10.0861290890013</v>
       </c>
     </row>
-    <row r="2617" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2617" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2617" t="s">
         <v>41</v>
       </c>
@@ -61240,7 +61240,7 @@
         <v>10.323759005323501</v>
       </c>
     </row>
-    <row r="2618" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2618" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2618" t="s">
         <v>32</v>
       </c>
@@ -61263,7 +61263,7 @@
         <v>10.1464279428772</v>
       </c>
     </row>
-    <row r="2619" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2619" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2619" t="s">
         <v>46</v>
       </c>
@@ -61286,7 +61286,7 @@
         <v>10.395672176439501</v>
       </c>
     </row>
-    <row r="2620" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2620" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2620" t="s">
         <v>34</v>
       </c>
@@ -61309,7 +61309,7 @@
         <v>10.443658362853499</v>
       </c>
     </row>
-    <row r="2621" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2621" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2621" t="s">
         <v>7</v>
       </c>
@@ -61355,7 +61355,7 @@
         <v>10.595281968876501</v>
       </c>
     </row>
-    <row r="2623" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2623" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2623" t="s">
         <v>34</v>
       </c>
@@ -61401,7 +61401,7 @@
         <v>11.102702373746601</v>
       </c>
     </row>
-    <row r="2625" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2625" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2625" t="s">
         <v>49</v>
       </c>
@@ -61424,7 +61424,7 @@
         <v>10.7582526462246</v>
       </c>
     </row>
-    <row r="2626" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2626" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2626" t="s">
         <v>21</v>
       </c>
@@ -61447,7 +61447,7 @@
         <v>10.9064201276129</v>
       </c>
     </row>
-    <row r="2627" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2627" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2627" t="s">
         <v>32</v>
       </c>
@@ -61470,7 +61470,7 @@
         <v>10.9590145542379</v>
       </c>
     </row>
-    <row r="2628" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2628" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2628" t="s">
         <v>16</v>
       </c>
@@ -61493,7 +61493,7 @@
         <v>10.676141625137801</v>
       </c>
     </row>
-    <row r="2629" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2629" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2629" t="s">
         <v>21</v>
       </c>
@@ -61516,7 +61516,7 @@
         <v>10.875201147565001</v>
       </c>
     </row>
-    <row r="2630" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2630" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2630" t="s">
         <v>44</v>
       </c>
@@ -61539,7 +61539,7 @@
         <v>10.900917392586701</v>
       </c>
     </row>
-    <row r="2631" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2631" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2631" t="s">
         <v>32</v>
       </c>
@@ -61585,7 +61585,7 @@
         <v>10.6573918009989</v>
       </c>
     </row>
-    <row r="2633" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2633" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2633" t="s">
         <v>7</v>
       </c>
@@ -61608,7 +61608,7 @@
         <v>10.989540481749</v>
       </c>
     </row>
-    <row r="2634" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2634" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2634" t="s">
         <v>33</v>
       </c>
@@ -61631,7 +61631,7 @@
         <v>10.9407495172862</v>
       </c>
     </row>
-    <row r="2635" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2635" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2635" t="s">
         <v>33</v>
       </c>
@@ -61654,7 +61654,7 @@
         <v>11.285388783732699</v>
       </c>
     </row>
-    <row r="2636" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2636" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2636" t="s">
         <v>49</v>
       </c>
@@ -61677,7 +61677,7 @@
         <v>11.1126054550676</v>
       </c>
     </row>
-    <row r="2637" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2637" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2637" t="s">
         <v>21</v>
       </c>
@@ -61723,7 +61723,7 @@
         <v>11.2498888883401</v>
       </c>
     </row>
-    <row r="2639" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2639" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2639" t="s">
         <v>16</v>
       </c>
@@ -61746,7 +61746,7 @@
         <v>10.9325202949731</v>
       </c>
     </row>
-    <row r="2640" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2640" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2640" t="s">
         <v>46</v>
       </c>
@@ -61769,7 +61769,7 @@
         <v>11.4581848475227</v>
       </c>
     </row>
-    <row r="2641" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2641" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2641" t="s">
         <v>21</v>
       </c>
@@ -61792,7 +61792,7 @@
         <v>11.1198021565134</v>
       </c>
     </row>
-    <row r="2642" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2642" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2642" t="s">
         <v>37</v>
       </c>
@@ -61815,7 +61815,7 @@
         <v>11.360017605620101</v>
       </c>
     </row>
-    <row r="2643" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2643" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2643" t="s">
         <v>43</v>
       </c>
@@ -61838,7 +61838,7 @@
         <v>11.057576588023201</v>
       </c>
     </row>
-    <row r="2644" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2644" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2644" t="s">
         <v>46</v>
       </c>
@@ -61861,7 +61861,7 @@
         <v>11.298229949863799</v>
       </c>
     </row>
-    <row r="2645" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2645" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2645" t="s">
         <v>45</v>
       </c>
@@ -61884,7 +61884,7 @@
         <v>11.248110952511</v>
       </c>
     </row>
-    <row r="2646" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2646" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2646" t="s">
         <v>37</v>
       </c>
@@ -61907,7 +61907,7 @@
         <v>11.3573764576155</v>
       </c>
     </row>
-    <row r="2647" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2647" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2647" t="s">
         <v>33</v>
       </c>
@@ -61930,7 +61930,7 @@
         <v>11.2445542374964</v>
       </c>
     </row>
-    <row r="2648" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2648" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2648" t="s">
         <v>46</v>
       </c>
@@ -61953,7 +61953,7 @@
         <v>11.6262633722103</v>
       </c>
     </row>
-    <row r="2649" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2649" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2649" t="s">
         <v>21</v>
       </c>
@@ -61976,7 +61976,7 @@
         <v>11.248555462813799</v>
       </c>
     </row>
-    <row r="2650" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2650" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2650" t="s">
         <v>21</v>
       </c>
@@ -61999,7 +61999,7 @@
         <v>11.6051712611232</v>
       </c>
     </row>
-    <row r="2651" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2651" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2651" t="s">
         <v>16</v>
       </c>
@@ -62068,7 +62068,7 @@
         <v>11.582314103839501</v>
       </c>
     </row>
-    <row r="2654" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2654" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2654" t="s">
         <v>44</v>
       </c>
@@ -62091,7 +62091,7 @@
         <v>11.433722053644599</v>
       </c>
     </row>
-    <row r="2655" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2655" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2655" t="s">
         <v>44</v>
       </c>
@@ -62114,7 +62114,7 @@
         <v>11.6520384482716</v>
       </c>
     </row>
-    <row r="2656" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2656" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2656" t="s">
         <v>47</v>
       </c>
@@ -62137,7 +62137,7 @@
         <v>11.5684916907952</v>
       </c>
     </row>
-    <row r="2657" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2657" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2657" t="s">
         <v>44</v>
       </c>
@@ -62160,7 +62160,7 @@
         <v>11.5723809131915</v>
       </c>
     </row>
-    <row r="2658" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2658" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2658" t="s">
         <v>21</v>
       </c>
@@ -62183,7 +62183,7 @@
         <v>11.690166808048501</v>
       </c>
     </row>
-    <row r="2659" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2659" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2659" t="s">
         <v>16</v>
       </c>
@@ -62206,7 +62206,7 @@
         <v>11.7698768047928</v>
       </c>
     </row>
-    <row r="2660" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2660" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2660" t="s">
         <v>49</v>
       </c>
@@ -62229,7 +62229,7 @@
         <v>12.0349491066643</v>
       </c>
     </row>
-    <row r="2661" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2661" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2661" t="s">
         <v>44</v>
       </c>
@@ -62252,7 +62252,7 @@
         <v>11.8105884696741</v>
       </c>
     </row>
-    <row r="2662" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2662" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2662" t="s">
         <v>31</v>
       </c>
@@ -62321,7 +62321,7 @@
         <v>11.9808180021232</v>
       </c>
     </row>
-    <row r="2665" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2665" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2665" t="s">
         <v>47</v>
       </c>
@@ -62344,7 +62344,7 @@
         <v>11.8498945142984</v>
       </c>
     </row>
-    <row r="2666" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2666" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2666" t="s">
         <v>21</v>
       </c>
@@ -62367,12 +62367,12 @@
         <v>12.004165943538</v>
       </c>
     </row>
-    <row r="2667" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2667" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2667" t="s">
         <v>48</v>
       </c>
       <c r="B2667" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C2667" t="s">
         <v>57</v>
@@ -62381,21 +62381,21 @@
         <v>56</v>
       </c>
       <c r="E2667">
-        <v>11.8207444774007</v>
+        <v>11.8680242669114</v>
       </c>
       <c r="F2667">
-        <v>5.1332251070842396</v>
+        <v>1.4035668847618199</v>
       </c>
       <c r="G2667">
-        <v>12.887202954869601</v>
-      </c>
-    </row>
-    <row r="2668" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11.9507321951418</v>
+      </c>
+    </row>
+    <row r="2668" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2668" t="s">
         <v>48</v>
       </c>
       <c r="B2668" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C2668" t="s">
         <v>57</v>
@@ -62404,21 +62404,21 @@
         <v>56</v>
       </c>
       <c r="E2668">
-        <v>11.8680242669114</v>
+        <v>11.874342087037901</v>
       </c>
       <c r="F2668">
-        <v>1.4035668847618199</v>
+        <v>3.0413812651490999</v>
       </c>
       <c r="G2668">
-        <v>11.9507321951418</v>
-      </c>
-    </row>
-    <row r="2669" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12.2576506721312</v>
+      </c>
+    </row>
+    <row r="2669" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2669" t="s">
         <v>48</v>
       </c>
       <c r="B2669" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C2669" t="s">
         <v>57</v>
@@ -62427,16 +62427,16 @@
         <v>56</v>
       </c>
       <c r="E2669">
-        <v>11.874342087037901</v>
+        <v>12.1626477380544</v>
       </c>
       <c r="F2669">
-        <v>3.0413812651490999</v>
+        <v>3.2202484376209202</v>
       </c>
       <c r="G2669">
-        <v>12.2576506721312</v>
-      </c>
-    </row>
-    <row r="2670" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12.581732790041199</v>
+      </c>
+    </row>
+    <row r="2670" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2670" t="s">
         <v>31</v>
       </c>
@@ -62459,7 +62459,7 @@
         <v>12.108261642366299</v>
       </c>
     </row>
-    <row r="2671" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2671" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2671" t="s">
         <v>44</v>
       </c>
@@ -62482,7 +62482,7 @@
         <v>12.251938622112</v>
       </c>
     </row>
-    <row r="2672" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2672" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2672" t="s">
         <v>19</v>
       </c>
@@ -62505,7 +62505,7 @@
         <v>12.166347027764701</v>
       </c>
     </row>
-    <row r="2673" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2673" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2673" t="s">
         <v>33</v>
       </c>
@@ -62551,7 +62551,7 @@
         <v>12.3012194517454</v>
       </c>
     </row>
-    <row r="2675" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2675" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2675" t="s">
         <v>48</v>
       </c>
@@ -62574,7 +62574,7 @@
         <v>12.8054675822478</v>
       </c>
     </row>
-    <row r="2676" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2676" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2676" t="s">
         <v>47</v>
       </c>
@@ -62597,7 +62597,7 @@
         <v>12.3109707172099</v>
       </c>
     </row>
-    <row r="2677" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2677" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2677" t="s">
         <v>31</v>
       </c>
@@ -62620,7 +62620,7 @@
         <v>12.449497981846401</v>
       </c>
     </row>
-    <row r="2678" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2678" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2678" t="s">
         <v>44</v>
       </c>
@@ -62643,7 +62643,7 @@
         <v>12.4759769156567</v>
       </c>
     </row>
-    <row r="2679" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2679" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2679" t="s">
         <v>19</v>
       </c>
@@ -62666,12 +62666,12 @@
         <v>12.898061869908901</v>
       </c>
     </row>
-    <row r="2680" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2680" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2680" t="s">
         <v>48</v>
       </c>
       <c r="B2680" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C2680" t="s">
         <v>57</v>
@@ -62680,16 +62680,16 @@
         <v>56</v>
       </c>
       <c r="E2680">
-        <v>12.1626477380544</v>
+        <v>11.8207444774007</v>
       </c>
       <c r="F2680">
-        <v>3.2202484376209202</v>
+        <v>5.1332251070842396</v>
       </c>
       <c r="G2680">
-        <v>12.581732790041199</v>
-      </c>
-    </row>
-    <row r="2681" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12.887202954869601</v>
+      </c>
+    </row>
+    <row r="2681" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2681" t="s">
         <v>43</v>
       </c>
@@ -62712,7 +62712,7 @@
         <v>12.4418648119966</v>
       </c>
     </row>
-    <row r="2682" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2682" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2682" t="s">
         <v>21</v>
       </c>
@@ -62735,7 +62735,7 @@
         <v>12.450702791408901</v>
       </c>
     </row>
-    <row r="2683" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2683" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2683" t="s">
         <v>47</v>
       </c>
@@ -62758,7 +62758,7 @@
         <v>12.9491312449909</v>
       </c>
     </row>
-    <row r="2684" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2684" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2684" t="s">
         <v>31</v>
       </c>
@@ -62781,7 +62781,7 @@
         <v>12.674778104566499</v>
       </c>
     </row>
-    <row r="2685" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2685" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2685" t="s">
         <v>47</v>
       </c>
@@ -62827,7 +62827,7 @@
         <v>12.3874936932375</v>
       </c>
     </row>
-    <row r="2687" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2687" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2687" t="s">
         <v>44</v>
       </c>
@@ -62850,7 +62850,7 @@
         <v>13.148003650744799</v>
       </c>
     </row>
-    <row r="2688" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2688" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2688" t="s">
         <v>31</v>
       </c>
@@ -62873,7 +62873,7 @@
         <v>12.8767231856555</v>
       </c>
     </row>
-    <row r="2689" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2689" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2689" t="s">
         <v>19</v>
       </c>
@@ -62896,7 +62896,7 @@
         <v>12.854571171377099</v>
       </c>
     </row>
-    <row r="2690" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2690" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2690" t="s">
         <v>19</v>
       </c>
@@ -62919,7 +62919,7 @@
         <v>13.149524706239299</v>
       </c>
     </row>
-    <row r="2691" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2691" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2691" t="s">
         <v>47</v>
       </c>
@@ -62942,7 +62942,7 @@
         <v>12.9510617325376</v>
       </c>
     </row>
-    <row r="2692" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2692" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2692" t="s">
         <v>31</v>
       </c>
@@ -62965,7 +62965,7 @@
         <v>12.998846102635399</v>
       </c>
     </row>
-    <row r="2693" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2693" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2693" t="s">
         <v>47</v>
       </c>
@@ -62988,7 +62988,7 @@
         <v>13.374228949737599</v>
       </c>
     </row>
-    <row r="2694" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2694" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2694" t="s">
         <v>44</v>
       </c>
@@ -63011,7 +63011,7 @@
         <v>13.239335330748199</v>
       </c>
     </row>
-    <row r="2695" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2695" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2695" t="s">
         <v>48</v>
       </c>
@@ -63034,7 +63034,7 @@
         <v>13.4354009988537</v>
       </c>
     </row>
-    <row r="2696" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2696" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2696" t="s">
         <v>47</v>
       </c>
@@ -63057,7 +63057,7 @@
         <v>12.7318498263213</v>
       </c>
     </row>
-    <row r="2697" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2697" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2697" t="s">
         <v>48</v>
       </c>
@@ -63103,7 +63103,7 @@
         <v>13.7422705547518</v>
       </c>
     </row>
-    <row r="2699" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2699" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2699" t="s">
         <v>45</v>
       </c>
@@ -63126,7 +63126,7 @@
         <v>14.4537192445404</v>
       </c>
     </row>
-    <row r="2700" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2700" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2700" t="s">
         <v>48</v>
       </c>
@@ -63149,7 +63149,7 @@
         <v>14.062716664997501</v>
       </c>
     </row>
-    <row r="2701" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2701" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2701" t="s">
         <v>47</v>
       </c>
@@ -63174,6 +63174,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G2701" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="r1i1p1f1"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="2">
       <filters>
         <filter val="All"/>
@@ -63184,7 +63189,7 @@
         <filter val="Annual"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2594:G2701">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2594:G2698">
       <sortCondition ref="E1:E2701"/>
     </sortState>
   </autoFilter>

</xml_diff>